<commit_message>
se arregla Carga.py y la clave de 4 digitos
</commit_message>
<xml_diff>
--- a/4-DESARROLLO/CARGA.xlsx
+++ b/4-DESARROLLO/CARGA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EVALF\4-DESARROLLO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A68F478-2881-4905-BD91-DE307D468016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A266D57F-6C78-4767-BB00-097B4AEA2437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{9BACD001-97DF-4BDB-BBD9-497BAC38CD66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{9BACD001-97DF-4BDB-BBD9-497BAC38CD66}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTOR" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="83">
   <si>
     <t>DNI</t>
   </si>
@@ -264,9 +264,6 @@
   </si>
   <si>
     <t>NUNCA, A VECES, SIEMPRE</t>
-  </si>
-  <si>
-    <t>NUNCA, A VECES SIEMPRE</t>
   </si>
   <si>
     <t>JOSE FERNANDO GALINDO SUAREZ</t>
@@ -709,13 +706,13 @@
         <v>19407970</v>
       </c>
       <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2">
+        <v>3147246</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="C2">
-        <v>3147246</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -723,13 +720,13 @@
         <v>19123456</v>
       </c>
       <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3">
+        <v>3147246</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="C3">
-        <v>3147246</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -745,7 +742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C02E86-6BAC-439D-AB6E-25BDF2E1ABBE}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -1314,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB65A05B-B8A0-478F-A387-6169927FB7F8}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1377,7 +1374,7 @@
         <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:2">

</xml_diff>